<commit_message>
updated api maturiteit lijst
</commit_message>
<xml_diff>
--- a/documenten/20191022 checklist_api_maturiteit.xlsx
+++ b/documenten/20191022 checklist_api_maturiteit.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicky\Documents\Netage\Rapporten\DIS-GEO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicky\git\disgeo-demo\documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F9993C-07FE-4AD8-A496-E9C20B62E59D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D13FCA5-E32A-49A8-BC13-7AEC8AD5661E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad1" sheetId="2" r:id="rId2"/>
+    <sheet name="Criteria" sheetId="1" r:id="rId1"/>
+    <sheet name="api's" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>Checklist API Maturiteit</t>
   </si>
@@ -109,15 +109,6 @@
     <t>Maturiteit per API</t>
   </si>
   <si>
-    <t>Is er verwijsbare documentatie van de begrippen beschikbaar?</t>
-  </si>
-  <si>
-    <t>Bevat de API alle benodige data/is de data compleet</t>
-  </si>
-  <si>
-    <t>De API stelt geen gebruiksbeperkende maatregelen?</t>
-  </si>
-  <si>
     <t>Opmerkingen</t>
   </si>
   <si>
@@ -182,13 +173,31 @@
   </si>
   <si>
     <t>Is er een data model beschikbaar</t>
+  </si>
+  <si>
+    <t>Dienst Uitvoerig Onderwijs API</t>
+  </si>
+  <si>
+    <t>Rijksdienst voor Cultureel Erfgoed API</t>
+  </si>
+  <si>
+    <t>Rijksdienst voor het Wegverkeer</t>
+  </si>
+  <si>
+    <t>De RCE biedt een API maar niet de mogelijkheid om een individueel monument te bevragen. Dit kan enkel voor een complete gemeente. Verder is er geen relatie tot data uit het kadaster en kan er niet geografisch worden gezocht.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duo biedt een goed gevulde API. Deze heeft geen relatie tot andere datasets en bevat geen geo informatie. </t>
+  </si>
+  <si>
+    <t>De RDW api bevat veel informatie. Echter is de informatie veel verspreid. Zo bevat de dataset over parkeervakken meer dan 5 tabellen, dit maakt het lastig bruikbaar. De RDW data bevat geo informatie maar de geo informatie is niet bevraagbaar in de API.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -212,8 +221,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,20 +238,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
-        <bgColor rgb="FF339966"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -395,21 +405,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="163" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="163" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="163" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -418,54 +416,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -850,316 +858,307 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" customWidth="1"/>
-    <col min="2" max="2" width="60.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="6" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="60.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:5" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="23" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="23"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="17"/>
+      <c r="D4" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="11" t="s">
-        <v>41</v>
+      <c r="C5" s="17"/>
+      <c r="D5" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="23"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="5"/>
       <c r="E7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
+      <c r="C9" s="15"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
         <v>5</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="17"/>
+      <c r="D10" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>6</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="11"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="5"/>
       <c r="E11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>9</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="11" t="s">
-        <v>44</v>
+      <c r="C14" s="24"/>
+      <c r="D14" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>10</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+      <c r="B15" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="24"/>
+      <c r="D15" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>11</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="20">
+      <c r="C16" s="24"/>
+      <c r="D16" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
         <v>12</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="11"/>
+      <c r="B17" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="5"/>
       <c r="E17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="31"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="13"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="11"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="15"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>13</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="11"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+      <c r="C20" s="17"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>14</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
+      <c r="C21" s="24"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>15</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="11" t="s">
-        <v>45</v>
+      <c r="C22" s="24"/>
+      <c r="D22" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="D23" s="19"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="19"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>16</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="11"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="5"/>
       <c r="E25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
         <v>17</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="10">
+      <c r="C26" s="17"/>
+      <c r="D26" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
         <v>18</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="11" t="s">
-        <v>47</v>
+      <c r="C27" s="17"/>
+      <c r="D27" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B3:C3"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B6:C6"/>
@@ -1176,6 +1175,15 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1184,139 +1192,206 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L8:L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="46.88671875" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
-    <col min="8" max="8" width="6.88671875" customWidth="1"/>
-    <col min="9" max="9" width="7.21875" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="34.33203125" customWidth="1"/>
-    <col min="14" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" customWidth="1"/>
+    <col min="12" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="87.5703125" customWidth="1"/>
+    <col min="21" max="1032" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="154.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:20" ht="154.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="7"/>
-      <c r="M2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3">
+    </row>
+    <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="B3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="B4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
+      <c r="B5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="27" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>